<commit_message>
desenvolvimento do sprint 6 e do relatorio final
</commit_message>
<xml_diff>
--- a/planilha tcc.xlsx
+++ b/planilha tcc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinnys2\Desktop\tcc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IFSP\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F641BB6C-79D6-4235-A633-CE1D0453CEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED7C54-B93F-4EA4-825E-1D3C10836EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
   <si>
     <t>Título do projeto:</t>
   </si>
@@ -200,16 +200,52 @@
     <t>Sprint 6</t>
   </si>
   <si>
-    <t>altera_dose</t>
-  </si>
-  <si>
-    <t>remove_dose</t>
-  </si>
-  <si>
     <t>criar_lote</t>
   </si>
   <si>
     <t>https://github.com/Vinnys2/tcc1.1</t>
+  </si>
+  <si>
+    <t>Início do desenvolvimento do relatório final</t>
+  </si>
+  <si>
+    <t>....</t>
+  </si>
+  <si>
+    <t>Aqui o inicio da criação do relatório, com introduções e ideias principais do tema.</t>
+  </si>
+  <si>
+    <t>agenda_dose</t>
+  </si>
+  <si>
+    <t>altera_lote</t>
+  </si>
+  <si>
+    <t>remove_lote</t>
+  </si>
+  <si>
+    <t>insere lote</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>fazer video</t>
+  </si>
+  <si>
+    <t>listar_lote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deu uns pequenos problemas na inicialização do banco, mas nada grave, acho que até domingo iremos conseguir resolver. </t>
+  </si>
+  <si>
+    <t>Sem problemas.</t>
+  </si>
+  <si>
+    <t>continuar relatório final</t>
+  </si>
+  <si>
+    <t>Fizemos algumas pesquisas e estamos indo bem.</t>
   </si>
 </sst>
 </file>
@@ -587,10 +623,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -768,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1285,7 +1321,7 @@
       </c>
       <c r="E48" s="20"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>44393</v>
       </c>
@@ -1300,7 +1336,7 @@
       </c>
       <c r="E49" s="20"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>44393</v>
       </c>
@@ -1315,7 +1351,7 @@
       </c>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>44393</v>
       </c>
@@ -1330,7 +1366,7 @@
       </c>
       <c r="E51" s="20"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>44393</v>
       </c>
@@ -1345,28 +1381,41 @@
       </c>
       <c r="E52" s="20"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>44402</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
         <v>58</v>
       </c>
@@ -1375,7 +1424,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -1392,65 +1441,112 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>44402</v>
+      </c>
       <c r="B58" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
+      <c r="C58" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>44402</v>
+      </c>
       <c r="B59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>44406</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C60" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>44407</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>44409</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="19"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>44410</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" s="7">
+        <v>44409</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1465,44 +1561,72 @@
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="A66" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="A67" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="B69" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="B70" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="B71" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
@@ -8010,7 +8134,10 @@
       <c r="E1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E53:H53"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="E41:G42"/>

</xml_diff>

<commit_message>
Arrumado erro de cadastro e alteracao de postos, relatorio final está em andamento (quase no final)
</commit_message>
<xml_diff>
--- a/planilha tcc.xlsx
+++ b/planilha tcc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IFSP\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED7C54-B93F-4EA4-825E-1D3C10836EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C8830D-9A05-4896-95DB-22C541A046D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="77">
   <si>
     <t>Título do projeto:</t>
   </si>
@@ -173,9 +173,6 @@
     <t>altera_local</t>
   </si>
   <si>
-    <t>a fazer.</t>
-  </si>
-  <si>
     <t>remove_local</t>
   </si>
   <si>
@@ -218,12 +215,6 @@
     <t>agenda_dose</t>
   </si>
   <si>
-    <t>altera_lote</t>
-  </si>
-  <si>
-    <t>remove_lote</t>
-  </si>
-  <si>
     <t>insere lote</t>
   </si>
   <si>
@@ -231,9 +222,6 @@
   </si>
   <si>
     <t>fazer video</t>
-  </si>
-  <si>
-    <t>listar_lote</t>
   </si>
   <si>
     <t xml:space="preserve">Deu uns pequenos problemas na inicialização do banco, mas nada grave, acho que até domingo iremos conseguir resolver. </t>
@@ -246,6 +234,24 @@
   </si>
   <si>
     <t>Fizemos algumas pesquisas e estamos indo bem.</t>
+  </si>
+  <si>
+    <t>Feito durante as férias!</t>
+  </si>
+  <si>
+    <t>Projeto concluído e apresentado completamente ao orientador.</t>
+  </si>
+  <si>
+    <t>O projeto foi concluido porém encontramos erros e estamos a resolver.</t>
+  </si>
+  <si>
+    <t>mudar o o menu para um menu responsivo</t>
+  </si>
+  <si>
+    <t>a fazer</t>
+  </si>
+  <si>
+    <t>...</t>
   </si>
 </sst>
 </file>
@@ -394,13 +400,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -623,10 +629,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -641,23 +647,23 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -804,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1110,7 +1116,7 @@
         <v>44378</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>37</v>
@@ -1119,7 +1125,7 @@
         <v>44388</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
@@ -1155,7 +1161,7 @@
         <v>44388</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1218,18 +1224,18 @@
       <c r="D41" s="7">
         <v>44388</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>44388</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>11</v>
@@ -1237,9 +1243,9 @@
       <c r="D42" s="7">
         <v>44388</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
@@ -1288,7 +1294,7 @@
         <v>44397</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,7 +1332,7 @@
         <v>44393</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>37</v>
@@ -1371,7 +1377,7 @@
         <v>44393</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>37</v>
@@ -1386,20 +1392,20 @@
         <v>44402</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
@@ -1417,7 +1423,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1454,18 +1460,18 @@
       <c r="D58" s="7">
         <v>44409</v>
       </c>
-      <c r="E58" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="E58" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>44402</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>37</v>
@@ -1474,7 +1480,7 @@
         <v>44409</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -1482,7 +1488,7 @@
         <v>44406</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>37</v>
@@ -1491,7 +1497,7 @@
         <v>44409</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1499,7 +1505,7 @@
         <v>44407</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>37</v>
@@ -1508,7 +1514,7 @@
         <v>44409</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -1516,7 +1522,7 @@
         <v>44409</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>37</v>
@@ -1524,17 +1530,17 @@
       <c r="D62" s="7">
         <v>44409</v>
       </c>
-      <c r="E62" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F62" s="19"/>
+      <c r="E62" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>44410</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>37</v>
@@ -1543,7 +1549,7 @@
         <v>44409</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -1553,23 +1559,25 @@
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -1586,107 +1594,131 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <v>44413</v>
+      </c>
       <c r="B68" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
-      <c r="B70" s="2" t="s">
-        <v>65</v>
+      <c r="B70" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
-      <c r="B71" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="6"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -8134,15 +8166,16 @@
       <c r="E1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E53:H53"/>
+  <mergeCells count="9">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="E41:G42"/>
     <mergeCell ref="E35:G36"/>
     <mergeCell ref="E46:E52"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E53:H53"/>
+    <mergeCell ref="E68:G68"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>